<commit_message>
Updated Part Names and digikey part names
</commit_message>
<xml_diff>
--- a/hardware/rev_a/audible_bom.xlsx
+++ b/hardware/rev_a/audible_bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Home\audiBLE\hardware\rev_a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amits_000\Desktop\audiBLE\hardware\rev_a\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,9 +98,6 @@
     <t>0402 Resistor</t>
   </si>
   <si>
-    <t>1276-1442-6-ND</t>
-  </si>
-  <si>
     <t>RHM10.0KCDCT-ND</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>LGA_CAV3</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
     <t>Linear Technology RMS-to-DC convert</t>
   </si>
   <si>
@@ -221,40 +215,46 @@
     <t>a</t>
   </si>
   <si>
-    <t>RHM1.0KCETR-ND</t>
-  </si>
-  <si>
-    <t>RHM14KCDTR-ND</t>
-  </si>
-  <si>
-    <t>RHM20.0KCDTR-ND</t>
-  </si>
-  <si>
-    <t>RHM47KCETR-ND</t>
-  </si>
-  <si>
-    <t>490-6318-2-ND</t>
-  </si>
-  <si>
     <t>1276-6804-1-ND</t>
   </si>
   <si>
-    <t>490-6281-2-ND</t>
-  </si>
-  <si>
     <t>MAX417ESA+-ND</t>
   </si>
   <si>
-    <t>497-6871-2-ND</t>
-  </si>
-  <si>
     <t>1428-1028-1-ND</t>
   </si>
   <si>
     <t>LTC1966CMS8#PBF-ND</t>
   </si>
   <si>
-    <t>FK3503010LTR-ND</t>
+    <t>RHM1.0KCECT-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>RHM14KCDCT-ND</t>
+  </si>
+  <si>
+    <t>RHM20.0KCDCT-ND</t>
+  </si>
+  <si>
+    <t>RHM47KCECT-ND</t>
+  </si>
+  <si>
+    <t>490-6318-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1442-1-ND</t>
+  </si>
+  <si>
+    <t>490-6281-1-ND</t>
+  </si>
+  <si>
+    <t>497-6871-1-ND</t>
+  </si>
+  <si>
+    <t>FK3503010LCT-ND</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,10 +308,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,22 +630,22 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -667,35 +674,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -710,18 +717,18 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -736,24 +743,24 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -762,24 +769,24 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -788,24 +795,24 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -814,24 +821,24 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -840,18 +847,18 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -866,24 +873,24 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -892,24 +899,24 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -918,169 +925,169 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C20" t="s">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C21" t="s">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C22" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>